<commit_message>
branch e hibridación, memoria hasta ultimo apartado
</commit_message>
<xml_diff>
--- a/Trabajo/results/branch-10.xlsx
+++ b/Trabajo/results/branch-10.xlsx
@@ -563,7 +563,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="3">
-        <v>1253801741500</v>
+        <v>127836377946</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -583,7 +583,7 @@
         <v>357.5283114706</v>
       </c>
       <c r="C5" s="3">
-        <v>14931.8288</v>
+        <v>10260.2478</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -603,7 +603,7 @@
         <v>14.1446846675</v>
       </c>
       <c r="C6" s="3">
-        <v>705.83293</v>
+        <v>344.180383</v>
       </c>
       <c r="D6" s="2">
         <v>0.000110504</v>
@@ -623,7 +623,7 @@
         <v>38.7550811373</v>
       </c>
       <c r="C7" s="3">
-        <v>69.282163</v>
+        <v>117.858539</v>
       </c>
       <c r="D7" s="3">
         <v>115.0819266667</v>
@@ -643,7 +643,7 @@
         <v>26.1708063235</v>
       </c>
       <c r="C8" s="3">
-        <v>60.466613</v>
+        <v>66.853517</v>
       </c>
       <c r="D8" s="3">
         <v>34.5970701961</v>
@@ -663,7 +663,7 @@
         <v>67.5254553529</v>
       </c>
       <c r="C9" s="3">
-        <v>410.78107</v>
+        <v>510.82979</v>
       </c>
       <c r="D9" s="2">
         <v>38.4805584314</v>
@@ -683,7 +683,7 @@
         <v>28.0813021569</v>
       </c>
       <c r="C10" s="3">
-        <v>64.38911400000001</v>
+        <v>121.271979</v>
       </c>
       <c r="D10" s="3">
         <v>29.8291998039</v>
@@ -703,7 +703,7 @@
         <v>220.6905729608</v>
       </c>
       <c r="C11" s="3">
-        <v>1267.12174</v>
+        <v>1598.4183</v>
       </c>
       <c r="D11" s="3">
         <v>193.7879727451</v>
@@ -723,7 +723,7 @@
         <v>1171.6547498039</v>
       </c>
       <c r="C12" s="3">
-        <v>1072.95406</v>
+        <v>927.39034</v>
       </c>
       <c r="D12" s="2">
         <v>359.6807647059</v>
@@ -743,7 +743,7 @@
         <v>97.0394383333</v>
       </c>
       <c r="C13" s="3">
-        <v>797.995826</v>
+        <v>491.459075</v>
       </c>
       <c r="D13" s="2">
         <v>0.0194194193</v>
@@ -763,7 +763,7 @@
         <v>252464.2766784314</v>
       </c>
       <c r="C14" s="3">
-        <v>82238359.677</v>
+        <v>82172205.13699999</v>
       </c>
       <c r="D14" s="2">
         <v>4.9310863431</v>
@@ -783,7 +783,7 @@
         <v>778.7868645098</v>
       </c>
       <c r="C15" s="3">
-        <v>5488.59304</v>
+        <v>8596.4746</v>
       </c>
       <c r="D15" s="2">
         <v>5.9881427451</v>
@@ -803,7 +803,7 @@
         <v>74.5243931373</v>
       </c>
       <c r="C16" s="3">
-        <v>188.227995</v>
+        <v>152.204531</v>
       </c>
       <c r="D16" s="2">
         <v>0.0523983308</v>
@@ -823,7 +823,7 @@
         <v>204.4903833922</v>
       </c>
       <c r="C17" s="3">
-        <v>3978.73395</v>
+        <v>4323.02753</v>
       </c>
       <c r="D17" s="2">
         <v>0.0606027963</v>
@@ -843,7 +843,7 @@
         <v>180.410618451</v>
       </c>
       <c r="C18" s="3">
-        <v>439.05691</v>
+        <v>474.12874</v>
       </c>
       <c r="D18" s="3">
         <v>456.0592137255</v>
@@ -863,7 +863,7 @@
         <v>89.6863405686</v>
       </c>
       <c r="C19" s="3">
-        <v>139.186411</v>
+        <v>130.203457</v>
       </c>
       <c r="D19" s="2">
         <v>23.5045311765</v>
@@ -883,7 +883,7 @@
         <v>1926.033136549</v>
       </c>
       <c r="C20" s="3">
-        <v>4558.3</v>
+        <v>3713.7039</v>
       </c>
       <c r="D20" s="2">
         <v>0.0362999907</v>
@@ -903,7 +903,7 @@
         <v>64.182199598</v>
       </c>
       <c r="C21" s="3">
-        <v>3722.50095</v>
+        <v>4044.47962</v>
       </c>
       <c r="D21" s="2">
         <v>0.0051923244</v>
@@ -923,7 +923,7 @@
         <v>128.3756979804</v>
       </c>
       <c r="C22" s="3">
-        <v>208.346877</v>
+        <v>244.75483</v>
       </c>
       <c r="D22" s="3">
         <v>383.6904686275</v>
@@ -943,7 +943,7 @@
         <v>176.942994549</v>
       </c>
       <c r="C23" s="3">
-        <v>264.1222</v>
+        <v>251.45151</v>
       </c>
       <c r="D23" s="3">
         <v>188.8937176471</v>
@@ -963,7 +963,7 @@
         <v>114.7547752745</v>
       </c>
       <c r="C24" s="3">
-        <v>1182.30648</v>
+        <v>1175.86616</v>
       </c>
       <c r="D24" s="3">
         <v>100.481</v>
@@ -983,7 +983,7 @@
         <v>342.7784139216</v>
       </c>
       <c r="C25" s="3">
-        <v>451.24866</v>
+        <v>491.98218</v>
       </c>
       <c r="D25" s="3">
         <v>809.7517235294</v>
@@ -1003,7 +1003,7 @@
         <v>345.9974841373</v>
       </c>
       <c r="C26" s="3">
-        <v>429.6628</v>
+        <v>388.93089</v>
       </c>
       <c r="D26" s="2">
         <v>100</v>
@@ -1023,7 +1023,7 @@
         <v>434.801705098</v>
       </c>
       <c r="C27" s="3">
-        <v>805.53621</v>
+        <v>867.29317</v>
       </c>
       <c r="D27" s="2">
         <v>404.0113156863</v>
@@ -1043,7 +1043,7 @@
         <v>504.7361672353</v>
       </c>
       <c r="C28" s="3">
-        <v>1397.21843</v>
+        <v>1338.37435</v>
       </c>
       <c r="D28" s="2">
         <v>270.5882352941</v>
@@ -1063,7 +1063,7 @@
         <v>419.7187245098</v>
       </c>
       <c r="C29" s="3">
-        <v>520.2679900000001</v>
+        <v>504.64666</v>
       </c>
       <c r="D29" s="2">
         <v>389.728327451</v>
@@ -1083,7 +1083,7 @@
         <v>546.8650154902</v>
       </c>
       <c r="C30" s="3">
-        <v>802.6557</v>
+        <v>661.22308</v>
       </c>
       <c r="D30" s="2">
         <v>351.7333098039</v>
@@ -1103,7 +1103,7 @@
         <v>375.1733578431</v>
       </c>
       <c r="C31" s="3">
-        <v>472.94261</v>
+        <v>491.39772</v>
       </c>
       <c r="D31" s="2">
         <v>237.5455352941</v>
@@ -1123,7 +1123,7 @@
         <v>2470924.30004804</v>
       </c>
       <c r="C32" s="2">
-        <v>5310163.715</v>
+        <v>4232030.437000001</v>
       </c>
       <c r="D32" s="3">
         <v>80512.17467254899</v>

</xml_diff>